<commit_message>
Formulario funcional pero con mal aspecto
</commit_message>
<xml_diff>
--- a/AppGestionUsuarios/Resources/ArchivoDePruebasOU.xlsx
+++ b/AppGestionUsuarios/Resources/ArchivoDePruebasOU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\ArchivosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2174241-DC42-470E-A2D3-699BE7CD2256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312BFBB-FFFB-4C1D-B25E-6292D80D3E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OU_PRINCIPAL" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="DEPARTAMENTO" sheetId="3" r:id="rId3"/>
     <sheet name="LUGAR_ENVIO" sheetId="4" r:id="rId4"/>
     <sheet name="PORTAL_EMPLEADO" sheetId="5" r:id="rId5"/>
-    <sheet name="DB" sheetId="6" r:id="rId6"/>
-    <sheet name="QUOTA" sheetId="7" r:id="rId7"/>
+    <sheet name="CUOTA" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="ALCALDIA_WIN10">OU_SECUNDARIA!$A$2:$A$6</definedName>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="205">
   <si>
     <t>OU_PRINCIPAL</t>
   </si>
@@ -645,24 +644,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>DB-BRONZE</t>
-  </si>
-  <si>
-    <t>DB_PLATA</t>
-  </si>
-  <si>
-    <t>DB_ORO</t>
-  </si>
-  <si>
-    <t>DB_DIAMANTE</t>
-  </si>
-  <si>
-    <t>QUOTA</t>
-  </si>
-  <si>
     <t>50MB</t>
   </si>
   <si>
@@ -676,13 +657,16 @@
   </si>
   <si>
     <t>10GB</t>
+  </si>
+  <si>
+    <t>CUOTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,16 +744,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF990000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF351C75"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -822,18 +801,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD966"/>
         <bgColor rgb="FFFFD966"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE06666"/>
-        <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
     <fill>
@@ -930,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -953,14 +920,10 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3982,7 +3945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
@@ -5590,7 +5553,7 @@
   <dimension ref="A1:J281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:O18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7179,60 +7142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7241,33 +7158,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>205</v>
+      <c r="A2" s="22" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>206</v>
+      <c r="A3" s="22" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>207</v>
+      <c r="A4" s="22" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>208</v>
+      <c r="A5" s="22" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>209</v>
+      <c r="A6" s="22" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Código funcional con creación de directorio con cuota de usuario
</commit_message>
<xml_diff>
--- a/AppGestionUsuarios/Resources/ArchivoDePruebasOU.xlsx
+++ b/AppGestionUsuarios/Resources/ArchivoDePruebasOU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\ArchivosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312BFBB-FFFB-4C1D-B25E-6292D80D3E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F303099-2907-46A7-80F9-5687BD711A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -644,22 +644,22 @@
     <t>No</t>
   </si>
   <si>
-    <t>50MB</t>
-  </si>
-  <si>
-    <t>1GB</t>
-  </si>
-  <si>
-    <t>2.5GB</t>
-  </si>
-  <si>
-    <t>5GB</t>
-  </si>
-  <si>
-    <t>10GB</t>
-  </si>
-  <si>
     <t>CUOTA</t>
+  </si>
+  <si>
+    <t>2500 (2.5 GB)</t>
+  </si>
+  <si>
+    <t>1000 (1 GB)</t>
+  </si>
+  <si>
+    <t>50 (50 MB)</t>
+  </si>
+  <si>
+    <t>5000 (5GB)</t>
+  </si>
+  <si>
+    <t>10000 (10GB)</t>
   </si>
 </sst>
 </file>
@@ -7149,7 +7149,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7159,32 +7159,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>